<commit_message>
reading the graphml file directly
</commit_message>
<xml_diff>
--- a/public_html/openai_nodes.xlsx
+++ b/public_html/openai_nodes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonzalo\Documents\PPStoryTeller\public_html\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CC0820-7D93-4134-BEF8-503A043E3E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3945D55-259F-42FA-98AA-FE131759FECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F0C70961-722B-4495-BF89-B3B1A2021BFC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F0C70961-722B-4495-BF89-B3B1A2021BFC}"/>
   </bookViews>
   <sheets>
     <sheet name="openai_nodes" sheetId="2" r:id="rId1"/>
@@ -722,8 +722,8 @@
       <xdr:row>51</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="type">
@@ -746,7 +746,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -800,8 +800,8 @@
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" Requires="sle15">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+      <mc:Choice Requires="sle15">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="category">
@@ -824,7 +824,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -1276,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6431C0DD-01AE-4D66-8281-23B3C289771E}">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+    <sheetView tabSelected="1" topLeftCell="P70" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="Z83" sqref="Z83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5372,14 +5372,15 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{3A4CF648-6AED-40f4-86FF-DC5316D8AED3}">
       <x14:slicerList xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main">
-        <x14:slicer r:id="rId3"/>
+        <x14:slicer r:id="rId4"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>